<commit_message>
Upd grafico a torta.
</commit_message>
<xml_diff>
--- a/Contabilita_2024.xlsx
+++ b/Contabilita_2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://customgroupspa-my.sharepoint.com/personal/s_lazzaro_custom_it/Documents/Desktop/Finance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.lazzaro\OneDrive - CUSTOM SPA\Desktop\Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_EEEEEFFFB5D9C40133FBBA4D2BAEA63DE3CF37EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{644352E4-507B-4C2F-828D-25BF27C0D97E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC4D85-850E-4258-B04B-49572BDB1F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gennaio" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="120">
   <si>
     <t>Entrate</t>
   </si>
@@ -608,7 +608,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,6 +649,2399 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Percentuale</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> spese / totale</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Febbraio!$H$34:$H$38</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Spesa totale diesel</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spesa totale "spesa"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spesa totale carne</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bolletta gas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bolletta luce</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Febbraio!$J$34:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.19649740527230267</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12086483252212139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4933089394410125E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.7219671602977916E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3BCB-473D-9604-1AB2CFB02354}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.6457171916010499"/>
+          <c:y val="0.2364683581219014"/>
+          <c:w val="0.33761614173228344"/>
+          <c:h val="0.5248869932925051"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Percentuale</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> spese / totale</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent6">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront">
+                  <a:rot lat="0" lon="0" rev="0"/>
+                </a:camera>
+                <a:lightRig rig="threePt" dir="t">
+                  <a:rot lat="0" lon="0" rev="1200000"/>
+                </a:lightRig>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="63500" h="25400"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Marzo!$H$33:$H$39</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Spesa totale diesel</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spesa totale "spesa"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spesa totale carne</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Spesa totale ristoranti</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Spesa totale bar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bolletta gas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bolletta luce</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Marzo!$J$33:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.7983928455706046E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11318935908236666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1438662432765209E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9486099410278011E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20065938694835073</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B02-43D7-BC8B-85929420EF5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.63748053368328961"/>
+          <c:y val="0.20000947798191893"/>
+          <c:w val="0.34585279965004373"/>
+          <c:h val="0.63947142023913672"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{339C2956-4B5D-98C9-AC3D-8D6FE0378D0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5112C5D7-9DC3-1920-9160-90A776EF336B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2439,8 +4832,8 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37:I38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3381,6 +5774,10 @@
         <f xml:space="preserve"> SUMIF(B:B, "Diesel golf",E:E)</f>
         <v>170.77</v>
       </c>
+      <c r="J34" s="33">
+        <f>I34/J9</f>
+        <v>0.19649740527230267</v>
+      </c>
       <c r="T34" s="1"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
@@ -3403,6 +5800,10 @@
         <f xml:space="preserve"> SUMIF(B:B, "Spesa",E:E)</f>
         <v>105.04</v>
       </c>
+      <c r="J35" s="33">
+        <f>I35/J9</f>
+        <v>0.12086483252212139</v>
+      </c>
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
@@ -3425,6 +5826,10 @@
         <f xml:space="preserve"> SUMIF(B:B, "Spesa carne",E:E)</f>
         <v>39.049999999999997</v>
       </c>
+      <c r="J36" s="33">
+        <f>I36/J9</f>
+        <v>4.4933089394410125E-2</v>
+      </c>
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
@@ -3447,6 +5852,10 @@
         <f>SUMIF(B:B, "Bolletta gas",E:E)</f>
         <v>0</v>
       </c>
+      <c r="J37" s="33">
+        <f>I37/J9</f>
+        <v>0</v>
+      </c>
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
@@ -3469,6 +5878,10 @@
         <f>SUMIF(B:B, "Bolletta luce",E:E)</f>
         <v>75.8</v>
       </c>
+      <c r="J38" s="33">
+        <f>I38/J9</f>
+        <v>8.7219671602977916E-2</v>
+      </c>
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
@@ -3485,6 +5898,7 @@
         <v>3</v>
       </c>
       <c r="I39" s="23"/>
+      <c r="J39" s="33"/>
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
@@ -3501,6 +5915,7 @@
         <v>10.86</v>
       </c>
       <c r="I40" s="23"/>
+      <c r="J40" s="33"/>
       <c r="T40" s="1"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
@@ -3624,6 +6039,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3632,8 +6048,8 @@
   <sheetPr codeName="Foglio3"/>
   <dimension ref="A1:W57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J33:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3743,7 +6159,7 @@
       <c r="C3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="6">
         <v>10</v>
       </c>
       <c r="H3" s="7" t="s">
@@ -3773,7 +6189,7 @@
       <c r="C4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="6">
         <v>22.98</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -3912,7 +6328,7 @@
       </c>
       <c r="I9" s="9">
         <f>SUM(E:E)</f>
-        <v>1136.8499999999999</v>
+        <v>1234.48</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="21" x14ac:dyDescent="0.3">
@@ -4515,7 +6931,11 @@
       </c>
       <c r="I33" s="9">
         <f xml:space="preserve"> SUMIF(B:B, "Diesel golf",E:E)</f>
-        <v>0</v>
+        <v>71.58</v>
+      </c>
+      <c r="J33" s="33">
+        <f>I33/I9</f>
+        <v>5.7983928455706046E-2</v>
       </c>
       <c r="T33" s="1"/>
     </row>
@@ -4537,7 +6957,11 @@
       </c>
       <c r="I34" s="9">
         <f>SUMIF(B:B, "Spesa",E:E)</f>
-        <v>124.67999999999999</v>
+        <v>139.72999999999999</v>
+      </c>
+      <c r="J34" s="33">
+        <f>I34/I9</f>
+        <v>0.11318935908236666</v>
       </c>
       <c r="T34" s="1"/>
     </row>
@@ -4561,6 +6985,10 @@
         <f xml:space="preserve"> SUMIF(B:B, "Spesa carne",E:E)</f>
         <v>0</v>
       </c>
+      <c r="J35" s="33">
+        <f>I35/I9</f>
+        <v>0</v>
+      </c>
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
@@ -4583,6 +7011,10 @@
         <f>SUMIF(B:B, "Ristoranti",E:E)</f>
         <v>63.5</v>
       </c>
+      <c r="J36" s="33">
+        <f>I36/I9</f>
+        <v>5.1438662432765209E-2</v>
+      </c>
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
@@ -4603,7 +7035,11 @@
       </c>
       <c r="I37" s="9">
         <f>SUMIF(B:B, "Bar",E:E)</f>
-        <v>31.4</v>
+        <v>36.4</v>
+      </c>
+      <c r="J37" s="33">
+        <f>I37/I9</f>
+        <v>2.9486099410278011E-2</v>
       </c>
       <c r="T37" s="1"/>
     </row>
@@ -4627,9 +7063,25 @@
         <f>SUMIF(B:B, "Bolletta gas",E:E)</f>
         <v>247.71</v>
       </c>
+      <c r="J38" s="33">
+        <f>I38/I9</f>
+        <v>0.20065938694835073</v>
+      </c>
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>45376</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="6">
+        <v>5.39</v>
+      </c>
       <c r="H39" s="5" t="s">
         <v>74</v>
       </c>
@@ -4637,21 +7089,74 @@
         <f>SUMIF(B:B, "Bolletta luce",E:E)</f>
         <v>0</v>
       </c>
+      <c r="J39" s="33">
+        <f>I39/I9</f>
+        <v>0</v>
+      </c>
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>45376</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="6">
+        <v>5</v>
+      </c>
       <c r="I40" s="23"/>
+      <c r="J40" s="33"/>
       <c r="T40" s="1"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>45376</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="6">
+        <v>6</v>
+      </c>
       <c r="I41" s="23"/>
       <c r="T41" s="1"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>45376</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="6">
+        <v>71.58</v>
+      </c>
       <c r="I42" s="23"/>
       <c r="T42" s="1"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>45376</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="6">
+        <v>9.66</v>
+      </c>
       <c r="I43" s="23"/>
       <c r="T43" s="1"/>
     </row>
@@ -4718,5 +7223,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>